<commit_message>
fit_round more on bezier & 3circle
</commit_message>
<xml_diff>
--- a/others/fit_round/data.xlsx
+++ b/others/fit_round/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\projects\Matlab\others\fit_round\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F5D5E0-0184-4974-8B35-E0E799D96B7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EAC043-7B27-4D5A-A6AA-4BFE812BF5CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11475" xr2:uid="{336476F3-AB51-4764-B7CE-F3806CE2B78A}"/>
   </bookViews>
@@ -19,6 +19,8 @@
     <sheet name="dd" sheetId="4" r:id="rId4"/>
     <sheet name="xx" sheetId="5" r:id="rId5"/>
     <sheet name="yy" sheetId="6" r:id="rId6"/>
+    <sheet name="measure" sheetId="7" r:id="rId7"/>
+    <sheet name="centered" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -382,7 +384,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,4 +763,402 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426F6196-662B-4123-A9C4-6C26ABBBD237}">
+  <dimension ref="A1:B37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>-21.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>-21.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.35355339059327401</v>
+      </c>
+      <c r="B3">
+        <v>-19.1403499549969</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.42426406871192801</v>
+      </c>
+      <c r="B4">
+        <v>-19.211060633115501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.5</v>
+      </c>
+      <c r="B5">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.8</v>
+      </c>
+      <c r="B6">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2.4041630560342599</v>
+      </c>
+      <c r="B8">
+        <v>-14.119891808572399</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2.4748737341529199</v>
+      </c>
+      <c r="B9">
+        <v>-14.190602486691001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2.5</v>
+      </c>
+      <c r="B10">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>-11.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>-11.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5.5154328932550696</v>
+      </c>
+      <c r="B13">
+        <v>-10.1600938339277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5.6</v>
+      </c>
+      <c r="B14">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5.6568542494923797</v>
+      </c>
+      <c r="B15">
+        <v>-10.301515190165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>9.3338095116624302</v>
+      </c>
+      <c r="B17">
+        <v>-6.9074026404695799</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>9.5459415460183905</v>
+      </c>
+      <c r="B18">
+        <v>-7.1195346748255499</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>-6.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>13</v>
+      </c>
+      <c r="B21">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>13.930003589375</v>
+      </c>
+      <c r="B23">
+        <v>-4.4325289063166604</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>14.142135623731001</v>
+      </c>
+      <c r="B24">
+        <v>-4.6446609406726296</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>15</v>
+      </c>
+      <c r="B26">
+        <v>-4.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>18.9504617357995</v>
+      </c>
+      <c r="B27">
+        <v>-2.3819192408756802</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>19.091883092036799</v>
+      </c>
+      <c r="B28">
+        <v>-2.5233405971129801</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>20</v>
+      </c>
+      <c r="B29">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>20.5</v>
+      </c>
+      <c r="B31">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>24.112341238461301</v>
+      </c>
+      <c r="B32">
+        <v>-0.47273093167199698</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>24.395183950935898</v>
+      </c>
+      <c r="B33">
+        <v>-0.75557364414661499</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>25</v>
+      </c>
+      <c r="B34">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>25</v>
+      </c>
+      <c r="B35">
+        <v>-1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>29.5</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>29.5</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC1AD018-95E9-4759-A4D6-D832659F61E1}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>-21.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.42593915310173402</v>
+      </c>
+      <c r="B2">
+        <v>-19.4504701960375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2.23580735803744</v>
+      </c>
+      <c r="B3">
+        <v>-14.662098859052699</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5.4620478571245696</v>
+      </c>
+      <c r="B4">
+        <v>-10.526934837348801</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>9.7199377644202105</v>
+      </c>
+      <c r="B5">
+        <v>-6.9317343288237803</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>14.012023202184301</v>
+      </c>
+      <c r="B6">
+        <v>-4.6295316411648804</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>19.708468965567299</v>
+      </c>
+      <c r="B7">
+        <v>-2.4810519675977298</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>24.6268812973493</v>
+      </c>
+      <c r="B8">
+        <v>-0.95707614395465301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>29.5</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>